<commit_message>
location and excel file changed
</commit_message>
<xml_diff>
--- a/src/assets/MSA Typ 2_example data.xlsx
+++ b/src/assets/MSA Typ 2_example data.xlsx
@@ -1,23 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10514"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamal\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maartenover/Documents/1 Business/QM Datalab/Javascript Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B33351-0D43-0540-8B71-2313055E3CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -59,7 +71,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -94,9 +109,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -115,7 +132,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -376,16 +393,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -396,401 +413,437 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
-        <v>1.8071952896774557</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C2" s="3">
+        <v>1.8069999999999999</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1">
-        <v>1.6288853193559516</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C3" s="3">
+        <v>1.629</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1">
-        <v>1.5248895204978679</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C4" s="3">
+        <v>1.5249999999999999</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
-        <v>1.7362101979315745</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C5" s="3">
+        <v>1.736</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1">
-        <v>1.5642104260662653</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C6" s="3">
+        <v>1.5640000000000001</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1">
-        <v>1.4169298199502902</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C7" s="3">
+        <v>1.417</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="1">
-        <v>1.5755888525986919</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C8" s="3">
+        <v>1.5760000000000001</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1">
-        <v>1.4625079545533803</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C9" s="3">
+        <v>1.4630000000000001</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="1">
-        <v>1.569390728882645</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C10" s="3">
+        <v>1.569</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1">
-        <v>1.587962659011305</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C11" s="3">
+        <v>1.5880000000000001</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="1">
-        <v>1.2471558105407914</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C12" s="3">
+        <v>1.2470000000000001</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="1">
-        <v>1.3606601862150769</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C13" s="3">
+        <v>1.361</v>
+      </c>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="1">
-        <v>1.5895236965496795</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C14" s="3">
+        <v>1.59</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="1">
-        <v>1.5578609825590364</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C15" s="3">
+        <v>1.5580000000000001</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="1">
-        <v>1.6460762402905076</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C16" s="3">
+        <v>1.6459999999999999</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="1">
-        <v>1.5763046962450973</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C17" s="3">
+        <v>1.5760000000000001</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="1">
-        <v>1.4813907047448427</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C18" s="3">
+        <v>1.4810000000000001</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="1">
-        <v>1.8212596036379876</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C19" s="3">
+        <v>1.821</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="1">
-        <v>1.5776992172265745</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C20" s="3">
+        <v>1.5780000000000001</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="1">
-        <v>1.6480228795057263</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C21" s="3">
+        <v>1.6479999999999999</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="1">
-        <v>1.3818287813156758</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C22" s="3">
+        <v>1.3819999999999999</v>
+      </c>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="1">
-        <v>1.5088477107673648</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C23" s="3">
+        <v>1.5089999999999999</v>
+      </c>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="1">
-        <v>1.2864370332757777</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C24" s="3">
+        <v>1.286</v>
+      </c>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="1">
-        <v>1.5383570314054442</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C25" s="3">
+        <v>1.538</v>
+      </c>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="1">
-        <v>1.6915668000513397</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C26" s="3">
+        <v>1.6919999999999999</v>
+      </c>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="1">
-        <v>1.6414035529693805</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C27" s="3">
+        <v>1.641</v>
+      </c>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="1">
-        <v>1.4624108193931367</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C28" s="3">
+        <v>1.462</v>
+      </c>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="1">
-        <v>1.709597080891099</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C29" s="3">
+        <v>1.71</v>
+      </c>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="1">
-        <v>1.6422699642429865</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C30" s="3">
+        <v>1.6419999999999999</v>
+      </c>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="1">
-        <v>1.6078903842223755</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C31" s="3">
+        <v>1.6080000000000001</v>
+      </c>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="1">
-        <v>1.5981711440132664</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C32" s="3">
+        <v>1.5980000000000001</v>
+      </c>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="1">
-        <v>1.4924183738471255</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C33" s="3">
+        <v>1.492</v>
+      </c>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="1">
-        <v>1.613647182105695</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C34" s="3">
+        <v>1.6140000000000001</v>
+      </c>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="1">
-        <v>1.5961926031422131</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C35" s="3">
+        <v>1.5960000000000001</v>
+      </c>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="1">
-        <v>1.5996133714848666</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C36" s="3">
+        <v>1.601</v>
+      </c>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="1">
-        <v>1.4382757115951275</v>
-      </c>
+      <c r="C37" s="3">
+        <v>1.4379999999999999</v>
+      </c>
+      <c r="D37" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>